<commit_message>
drudes model implementation start
</commit_message>
<xml_diff>
--- a/project_code/linux_performance.xlsx
+++ b/project_code/linux_performance.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="257"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="257"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Size change" sheetId="1" r:id="rId1"/>
+    <sheet name="maxTime change" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Performance Analysis</t>
   </si>
@@ -64,24 +64,50 @@
   <si>
     <t>C++ (linux)</t>
   </si>
+  <si>
+    <t>percentage reduction</t>
+  </si>
+  <si>
+    <t>complexity factor</t>
+  </si>
+  <si>
+    <t>(tradeoff)</t>
+  </si>
+  <si>
+    <t>20 (matlab)</t>
+  </si>
+  <si>
+    <t>2 (C++)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,22 +122,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -218,7 +254,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$3</c:f>
+              <c:f>'Size change'!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -243,7 +279,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$18</c:f>
+              <c:f>'Size change'!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -297,7 +333,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$4:$J$18</c:f>
+              <c:f>'Size change'!$J$4:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -356,7 +392,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$3</c:f>
+              <c:f>'Size change'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -379,7 +415,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$18</c:f>
+              <c:f>'Size change'!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -433,7 +469,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$18</c:f>
+              <c:f>'Size change'!$D$4:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -492,7 +528,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$3</c:f>
+              <c:f>'Size change'!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -515,7 +551,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$18</c:f>
+              <c:f>'Size change'!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -569,7 +605,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$18</c:f>
+              <c:f>'Size change'!$F$4:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -628,7 +664,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$3</c:f>
+              <c:f>'Size change'!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -651,7 +687,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$18</c:f>
+              <c:f>'Size change'!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -705,7 +741,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$4:$H$18</c:f>
+              <c:f>'Size change'!$H$4:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -764,7 +800,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$3</c:f>
+              <c:f>'Size change'!$L$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -789,7 +825,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$18</c:f>
+              <c:f>'Size change'!$B$4:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -843,7 +879,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$18</c:f>
+              <c:f>'Size change'!$L$4:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -905,11 +941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="503548128"/>
-        <c:axId val="503545384"/>
+        <c:axId val="191571080"/>
+        <c:axId val="191613104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="503548128"/>
+        <c:axId val="191571080"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1025,12 +1061,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="503545384"/>
+        <c:crossAx val="191613104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="503545384"/>
+        <c:axId val="191613104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5800"/>
@@ -1149,7 +1185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="503548128"/>
+        <c:crossAx val="191571080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1796,16 +1832,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2090,13 +2126,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="11.5703125"/>
     <col min="4" max="5" width="17.28515625"/>
@@ -2107,16 +2143,38 @@
     <col min="10" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
     <row r="3" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
@@ -2130,13 +2188,13 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
@@ -2145,43 +2203,43 @@
       <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>1024</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <f>POWER(2,10)</f>
         <v>1024</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>0.125969</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
         <v>3.9460000000000002E-2</v>
       </c>
       <c r="E4" s="5">
         <v>4.2118000000000003E-2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <v>1.1341000000000001</v>
       </c>
       <c r="G4" s="5">
         <v>0.52138799999999996</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="2">
         <v>1.2706500000000001</v>
       </c>
       <c r="I4" s="5">
@@ -2190,41 +2248,39 @@
       <c r="J4" s="5">
         <v>0.59134200000000003</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="2">
         <v>1.3490800000000001</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="2">
         <v>0.13200700000000001</v>
       </c>
       <c r="M4" s="5">
         <v>7.7004000000000003E-2</v>
       </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5">
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
         <f>POWER(2,11)</f>
         <v>2048</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>0.22636700000000001</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <v>6.8043000000000006E-2</v>
       </c>
       <c r="E5" s="5">
         <v>6.4954999999999999E-2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="2">
         <v>0.86843199999999998</v>
       </c>
       <c r="G5" s="5">
         <v>0.62354600000000004</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="2">
         <v>1.11433</v>
       </c>
       <c r="I5" s="5">
@@ -2233,41 +2289,39 @@
       <c r="J5" s="5">
         <v>0.99970700000000001</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="2">
         <v>1.8951100000000001</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="2">
         <v>0.24501400000000001</v>
       </c>
       <c r="M5" s="5">
         <v>0.150009</v>
       </c>
-      <c r="N5" s="5">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5">
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
         <f>POWER(2,12)</f>
         <v>4096</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>0.91653300000000004</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>0.134355</v>
       </c>
       <c r="E6" s="5">
         <v>0.131297</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <v>1.2091700000000001</v>
       </c>
       <c r="G6" s="5">
         <v>0.98717299999999997</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="2">
         <v>1.29518</v>
       </c>
       <c r="I6" s="5">
@@ -2276,41 +2330,39 @@
       <c r="J6" s="5">
         <v>1.7086330000000001</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="2">
         <v>3.0511699999999999</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="2">
         <v>0.48402800000000001</v>
       </c>
       <c r="M6" s="5">
         <v>0.29901699999999998</v>
       </c>
-      <c r="N6" s="5">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5">
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
         <f>POWER(2,13)</f>
         <v>8192</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>3.0965400000000001</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="2">
         <v>0.263629</v>
       </c>
       <c r="E7" s="5">
         <v>0.25674599999999997</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <v>1.8743000000000001</v>
       </c>
       <c r="G7" s="5">
         <v>1.75437</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="2">
         <v>1.2845299999999999</v>
       </c>
       <c r="I7" s="5">
@@ -2319,41 +2371,39 @@
       <c r="J7" s="5">
         <v>3.3255379999999999</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="2">
         <v>5.1683000000000003</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="2">
         <v>1.0750599999999999</v>
       </c>
       <c r="M7" s="5">
         <v>0.61103499999999999</v>
       </c>
-      <c r="N7" s="5">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5">
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
         <f>POWER(2,14)</f>
         <v>16384</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>7.5690799999999996</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="2">
         <v>0.50695900000000005</v>
       </c>
       <c r="E8" s="5">
         <v>0.49728499999999998</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="2">
         <v>3.1196600000000001</v>
       </c>
       <c r="G8" s="5">
         <v>3.2157100000000001</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="2">
         <v>1.9201999999999999</v>
       </c>
       <c r="I8" s="5">
@@ -2362,41 +2412,39 @@
       <c r="J8" s="5">
         <v>4.9397060000000002</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="2">
         <v>6.55037</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="2">
         <v>1.9731099999999999</v>
       </c>
       <c r="M8" s="5">
         <v>1.0810599999999999</v>
       </c>
-      <c r="N8" s="5">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5">
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
         <f>POWER(2,15)</f>
         <v>32768</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>11.933</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>1.0148900000000001</v>
       </c>
       <c r="E9" s="5">
         <v>0.98334200000000005</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="2">
         <v>5.8561500000000004</v>
       </c>
       <c r="G9" s="5">
         <v>5.81562</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="2">
         <v>2.2463199999999999</v>
       </c>
       <c r="I9" s="5">
@@ -2405,41 +2453,39 @@
       <c r="J9" s="5">
         <v>8.0052529999999997</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="2">
         <v>13.597799999999999</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="2">
         <v>4.6592700000000002</v>
       </c>
       <c r="M9" s="5">
         <v>1.96411</v>
       </c>
-      <c r="N9" s="5">
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5">
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2">
         <f>POWER(2,16)</f>
         <v>65536</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>26.1995</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="2">
         <v>2.08996</v>
       </c>
       <c r="E10" s="5">
         <v>1.99203</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="2">
         <v>11.516299999999999</v>
       </c>
       <c r="G10" s="5">
         <v>11.028499999999999</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="2">
         <v>3.2987099999999998</v>
       </c>
       <c r="I10" s="5">
@@ -2448,41 +2494,39 @@
       <c r="J10" s="5">
         <v>18.160551000000002</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="2">
         <v>25.7075</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="2">
         <v>7.2584200000000001</v>
       </c>
       <c r="M10" s="5">
         <v>2.2961299999999998</v>
       </c>
-      <c r="N10" s="5">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5">
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2">
         <f>POWER(2,17)</f>
         <v>131072</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>52.891599999999997</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="2">
         <v>4.2423000000000002</v>
       </c>
       <c r="E11" s="5">
         <v>4.0933700000000002</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="2">
         <v>23.9191</v>
       </c>
       <c r="G11" s="5">
         <v>22.452500000000001</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="2">
         <v>5.1193900000000001</v>
       </c>
       <c r="I11" s="5">
@@ -2491,41 +2535,39 @@
       <c r="J11" s="5">
         <v>38.673577999999999</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="2">
         <v>87.941000000000003</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="2">
         <v>16.812999999999999</v>
       </c>
       <c r="M11" s="5">
         <v>4.4512499999999999</v>
       </c>
-      <c r="N11" s="5">
-        <v>3150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5">
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2">
         <f>POWER(2,18)</f>
         <v>262144</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <v>106.19799999999999</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="2">
         <v>8.4781399999999998</v>
       </c>
       <c r="E12" s="5">
         <v>8.2889999999999997</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <v>45.676600000000001</v>
       </c>
       <c r="G12" s="5">
         <v>46.064900000000002</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="2">
         <v>7.8305400000000001</v>
       </c>
       <c r="I12" s="5">
@@ -2534,41 +2576,39 @@
       <c r="J12" s="5">
         <v>79.686227000000002</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="2">
         <v>180.43899999999999</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="2">
         <v>32.554900000000004</v>
       </c>
       <c r="M12" s="5">
         <v>8.9255099999999992</v>
       </c>
-      <c r="N12" s="5">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5">
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
         <f>POWER(2,19)</f>
         <v>524288</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="2">
         <v>232.041</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="2">
         <v>17.034300000000002</v>
       </c>
       <c r="E13" s="5">
         <v>16.767099999999999</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="2">
         <v>91.505799999999994</v>
       </c>
       <c r="G13" s="5">
         <v>93.268000000000001</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="2">
         <v>12.8775</v>
       </c>
       <c r="I13" s="5">
@@ -2577,41 +2617,39 @@
       <c r="J13" s="5">
         <v>161.60210799999999</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="2">
         <v>327.47899999999998</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="2">
         <v>60.508499999999998</v>
       </c>
       <c r="M13" s="5">
         <v>17.827000000000002</v>
       </c>
-      <c r="N13" s="5">
-        <v>4050</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5">
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
         <f>POWER(2,20)</f>
         <v>1048576</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="2">
         <v>379.31700000000001</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="2">
         <v>33.955199999999998</v>
       </c>
       <c r="E14" s="5">
         <v>33.898400000000002</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="2">
         <v>183.49</v>
       </c>
       <c r="G14" s="5">
         <v>195.42400000000001</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="2">
         <v>22.6828</v>
       </c>
       <c r="I14" s="5">
@@ -2620,39 +2658,37 @@
       <c r="J14" s="5">
         <v>325.64582899999999</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="2">
         <v>534.47400000000005</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="2">
         <v>101.46899999999999</v>
       </c>
       <c r="M14" s="5">
         <v>35.996099999999998</v>
       </c>
-      <c r="N14" s="5">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2">
         <f>POWER(2,21)</f>
         <v>2097152</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>68.629800000000003</v>
       </c>
       <c r="E15" s="5">
         <v>67.221299999999999</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="2">
         <v>362.21100000000001</v>
       </c>
       <c r="G15" s="5">
         <v>376.80200000000002</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="2">
         <v>48.275100000000002</v>
       </c>
       <c r="I15" s="5">
@@ -2661,39 +2697,37 @@
       <c r="J15" s="5">
         <v>653.14065500000004</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="2">
         <v>1199.92</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="2">
         <v>266.48899999999998</v>
       </c>
       <c r="M15" s="5">
         <v>71.927099999999996</v>
       </c>
-      <c r="N15" s="5">
-        <v>4950</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5">
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2">
         <f>POWER(2,22)</f>
         <v>4194304</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
         <v>137.74600000000001</v>
       </c>
       <c r="E16" s="5">
         <v>136.96</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="2">
         <v>740.91099999999994</v>
       </c>
       <c r="G16" s="5">
         <v>772.07820000000004</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="2">
         <v>83.738900000000001</v>
       </c>
       <c r="I16" s="5">
@@ -2702,37 +2736,35 @@
       <c r="J16" s="5">
         <v>1322.5068140000001</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2">
         <v>489.697</v>
       </c>
       <c r="M16" s="5">
         <v>145.30500000000001</v>
       </c>
-      <c r="N16" s="5">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5">
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2">
         <f>POWER(2,23)</f>
         <v>8388608</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
         <v>275.38299999999998</v>
       </c>
       <c r="E17" s="5">
         <v>279.14499999999998</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="2">
         <v>1523.82</v>
       </c>
       <c r="G17" s="5">
         <v>1592.704</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="2">
         <v>176.589</v>
       </c>
       <c r="I17" s="5">
@@ -2741,37 +2773,35 @@
       <c r="J17" s="5">
         <v>2653.2642930000002</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2">
         <v>650.42100000000005</v>
       </c>
       <c r="M17" s="5">
         <v>291.75</v>
       </c>
-      <c r="N17" s="5">
-        <v>5850</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5">
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2">
         <f>POWER(2,24)</f>
         <v>16777216</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
         <v>575.76199999999994</v>
       </c>
       <c r="E18" s="5">
         <v>546.10400000000004</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="2">
         <v>3116.27</v>
       </c>
       <c r="G18" s="5">
         <v>3218.9009999999998</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="2">
         <v>328.01600000000002</v>
       </c>
       <c r="I18" s="5">
@@ -2780,43 +2810,309 @@
       <c r="J18" s="5">
         <v>5586.3581999999997</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2">
         <v>880.65899999999999</v>
       </c>
       <c r="M18" s="5">
         <v>588.15</v>
       </c>
-      <c r="N18" s="5">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:M2"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1025" width="11.5703125"/>
-  </cols>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <f>POWER(2,13)</f>
+        <v>8192</v>
+      </c>
+      <c r="B4" s="2">
+        <f>POWER(2,10)</f>
+        <v>1024</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.458831</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.77404399999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
+        <f>POWER(2,11)</f>
+        <v>2048</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7.1675139999999997</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.0441199999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
+        <f>POWER(2,12)</f>
+        <v>4096</v>
+      </c>
+      <c r="C6" s="2">
+        <v>12.239991</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.5611999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
+        <f>POWER(2,13)</f>
+        <v>8192</v>
+      </c>
+      <c r="C7" s="2">
+        <v>22.387522000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5.0122900000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
+        <f>POWER(2,14)</f>
+        <v>16384</v>
+      </c>
+      <c r="C8" s="2">
+        <v>67.892375999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>13.627800000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
+        <f>POWER(2,15)</f>
+        <v>32768</v>
+      </c>
+      <c r="C9" s="2">
+        <v>183.19263699999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>32.342799999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2">
+        <f>POWER(2,16)</f>
+        <v>65536</v>
+      </c>
+      <c r="C10" s="2">
+        <v>366.53059000000002</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1420.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2">
+        <f>POWER(2,17)</f>
+        <v>131072</v>
+      </c>
+      <c r="C11" s="2">
+        <v>575.89189799999997</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2875.21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2">
+        <f>POWER(2,18)</f>
+        <v>262144</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1382.9813839999999</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <f>POWER(2,19)</f>
+        <v>524288</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3285.1002020000001</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
+        <f>POWER(2,20)</f>
+        <v>1048576</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6715.9296670000003</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2">
+        <f>POWER(2,21)</f>
+        <v>2097152</v>
+      </c>
+      <c r="C15" s="2">
+        <v>11790.73609</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2">
+        <f>POWER(2,22)</f>
+        <v>4194304</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2">
+        <f>POWER(2,23)</f>
+        <v>8388608</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2">
+        <f>POWER(2,24)</f>
+        <v>16777216</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M2"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -2831,7 +3127,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="11.5703125"/>
   </cols>

</xml_diff>

<commit_message>
added drudes model Matlab/drudes.m
</commit_message>
<xml_diff>
--- a/project_code/linux_performance.xlsx
+++ b/project_code/linux_performance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="257"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="257"/>
   </bookViews>
   <sheets>
     <sheet name="Size change" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Performance Analysis</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>2 (C++)</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -941,13 +944,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191571080"/>
-        <c:axId val="191613104"/>
+        <c:axId val="239184472"/>
+        <c:axId val="238641536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="191571080"/>
+        <c:axId val="239184472"/>
         <c:scaling>
-          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
           <c:max val="27772160"/>
           <c:min val="1024"/>
@@ -1061,12 +1063,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191613104"/>
+        <c:crossAx val="238641536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191613104"/>
+        <c:axId val="238641536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5800"/>
@@ -1185,7 +1187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191571080"/>
+        <c:crossAx val="239184472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2126,10 +2128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2838,6 +2840,11 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J25" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J47" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>